<commit_message>
Centro- Topologia SW & PC Agregadas
</commit_message>
<xml_diff>
--- a/Docs/Tablas_Configuracion.xlsx
+++ b/Docs/Tablas_Configuracion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carl0\Desktop\Redes_Topo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FCF0C1-3DEC-49BF-8C75-BBA1A17AED50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D9E4D0-61E2-486B-82FA-B932081D92C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="-120" windowWidth="19590" windowHeight="11760" activeTab="1" xr2:uid="{337CC305-E2FF-4851-B46B-E00B2B44DC7A}"/>
   </bookViews>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>RED Corporativa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>130.45.0.0/16</t>
   </si>
@@ -53,13 +50,55 @@
   </si>
   <si>
     <t>P. # 1 Conectado a Router Centro</t>
+  </si>
+  <si>
+    <t>Dispositivo</t>
+  </si>
+  <si>
+    <t>Interfaz</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>RT_Bajas</t>
+  </si>
+  <si>
+    <t>RT_Noroeste</t>
+  </si>
+  <si>
+    <t>RT_Norte</t>
+  </si>
+  <si>
+    <t>RT_Centro</t>
+  </si>
+  <si>
+    <t>RT_Occidente</t>
+  </si>
+  <si>
+    <t>RT_Sureste</t>
+  </si>
+  <si>
+    <t>NOROESTE</t>
+  </si>
+  <si>
+    <t>CENTRO</t>
+  </si>
+  <si>
+    <t>Dominio</t>
+  </si>
+  <si>
+    <t>ramoso.com.mx</t>
+  </si>
+  <si>
+    <t>Red Corporativa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,35 +106,277 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,25 +691,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296807A8-A579-4B29-B76D-75FDD49B7475}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="27" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -437,79 +782,154 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6566E889-5BE1-4972-9A05-349D38C34B9F}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D14" sqref="A2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A3" s="14">
+        <v>10</v>
+      </c>
+      <c r="B3" s="15">
+        <v>2</v>
+      </c>
+      <c r="C3" s="16">
+        <v>6</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A4" s="14">
+        <v>15</v>
+      </c>
+      <c r="B4" s="15">
+        <v>7</v>
+      </c>
+      <c r="C4" s="16">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A5" s="14">
+        <v>20</v>
+      </c>
+      <c r="B5" s="15">
+        <v>13</v>
+      </c>
+      <c r="C5" s="16">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="17">
+        <v>90</v>
+      </c>
+      <c r="B6" s="18">
+        <v>19</v>
+      </c>
+      <c r="C6" s="19">
+        <v>24</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C10" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A11" s="14">
+        <v>30</v>
+      </c>
+      <c r="B11" s="15">
+        <v>2</v>
+      </c>
+      <c r="C11" s="16">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="D11" s="23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A12" s="14">
+        <v>35</v>
+      </c>
+      <c r="B12" s="15">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C12" s="16">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="13" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="A13" s="14">
+        <v>40</v>
+      </c>
+      <c r="B13" s="15">
         <v>13</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C13" s="16">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>90</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="17">
+        <v>95</v>
+      </c>
+      <c r="B14" s="18">
         <v>19</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C14" s="19">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
+      <c r="D14" s="23" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VTP Noroeste Configuradads V1
</commit_message>
<xml_diff>
--- a/Docs/Tablas_Configuracion.xlsx
+++ b/Docs/Tablas_Configuracion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carl0\Desktop\Redes_Topo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D9E4D0-61E2-486B-82FA-B932081D92C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F7B72E-8615-41D0-9FD9-74A00EC9ED0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="-120" windowWidth="19590" windowHeight="11760" activeTab="1" xr2:uid="{337CC305-E2FF-4851-B46B-E00B2B44DC7A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>130.45.0.0/16</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>Red Corporativa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130.45.1.1 </t>
+  </si>
+  <si>
+    <t>130.45.43.1</t>
+  </si>
+  <si>
+    <t>130.45.85.1</t>
+  </si>
+  <si>
+    <t>130.45.128.1</t>
+  </si>
+  <si>
+    <t>130.45.225.1</t>
+  </si>
+  <si>
+    <t>130.45.172.1</t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -198,17 +216,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -326,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,15 +347,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,22 +367,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -694,14 +700,14 @@
   <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.28515625" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
@@ -722,58 +728,70 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="27" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="25"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -784,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6566E889-5BE1-4972-9A05-349D38C34B9F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D14" sqref="A2:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,138 +815,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <v>10</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>2</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>6</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <v>15</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>7</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>12</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>20</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>13</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>18</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>90</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <v>19</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>24</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>30</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>2</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>6</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>35</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>7</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>40</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>13</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="17">
+      <c r="A14" s="16">
         <v>95</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>19</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="18">
         <v>24</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nororeste- VLANs & Router on Stick, Listo.
</commit_message>
<xml_diff>
--- a/Docs/Tablas_Configuracion.xlsx
+++ b/Docs/Tablas_Configuracion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carl0\Desktop\Redes_Topo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F7B72E-8615-41D0-9FD9-74A00EC9ED0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB75EB7F-3C85-4D79-B34A-1785ACD3E40B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="-120" windowWidth="19590" windowHeight="11760" activeTab="1" xr2:uid="{337CC305-E2FF-4851-B46B-E00B2B44DC7A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>130.45.0.0/16</t>
   </si>
@@ -110,6 +110,48 @@
   </si>
   <si>
     <t>130.45.172.1</t>
+  </si>
+  <si>
+    <t>IP Network</t>
+  </si>
+  <si>
+    <t>Mascara</t>
+  </si>
+  <si>
+    <t>130.45.43.1/26</t>
+  </si>
+  <si>
+    <t>130.45.43.65/26</t>
+  </si>
+  <si>
+    <t>130.45.43.129/26</t>
+  </si>
+  <si>
+    <t>130.45.43.193/26</t>
+  </si>
+  <si>
+    <t>255.255.255.192</t>
+  </si>
+  <si>
+    <t>g0/0.10</t>
+  </si>
+  <si>
+    <t>g0/0.15</t>
+  </si>
+  <si>
+    <t>g0/0.20</t>
+  </si>
+  <si>
+    <t>g0/0.90</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>ROUTER</t>
+  </si>
+  <si>
+    <t>Sub-Interfaz</t>
   </si>
 </sst>
 </file>
@@ -126,13 +168,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -173,6 +208,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -188,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -329,60 +372,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,7 +842,7 @@
       <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
@@ -800,26 +905,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6566E889-5BE1-4972-9A05-349D38C34B9F}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="27.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="B1" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -829,9 +944,18 @@
       <c r="C2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="D2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="13">
         <v>10</v>
       </c>
@@ -841,11 +965,20 @@
       <c r="C3" s="15">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="13">
         <v>15</v>
       </c>
@@ -855,9 +988,18 @@
       <c r="C4" s="15">
         <v>12</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="D4" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="13">
         <v>20</v>
       </c>
@@ -867,9 +1009,18 @@
       <c r="C5" s="15">
         <v>18</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="16">
         <v>90</v>
       </c>
@@ -879,17 +1030,26 @@
       <c r="C6" s="18">
         <v>24</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:4" ht="23.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+    <row r="8" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="9" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" s="19" t="s">
         <v>1</v>
       </c>
@@ -900,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
         <v>30</v>
       </c>
@@ -910,11 +1070,11 @@
       <c r="C11" s="15">
         <v>6</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="G11" s="22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="13">
         <v>35</v>
       </c>
@@ -925,7 +1085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
         <v>40</v>
       </c>
@@ -936,7 +1096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="16">
         <v>95</v>
       </c>
@@ -946,11 +1106,16 @@
       <c r="C14" s="18">
         <v>24</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="G14" s="22" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RIP funcionando entre Noroeste & Centro
</commit_message>
<xml_diff>
--- a/Docs/Tablas_Configuracion.xlsx
+++ b/Docs/Tablas_Configuracion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carl0\Desktop\Redes_Topo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB75EB7F-3C85-4D79-B34A-1785ACD3E40B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0399341A-06F4-4E98-9D1F-35D6F8C7EB69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="-120" windowWidth="19590" windowHeight="11760" activeTab="1" xr2:uid="{337CC305-E2FF-4851-B46B-E00B2B44DC7A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>130.45.0.0/16</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>Sub-Interfaz</t>
+  </si>
+  <si>
+    <t>g0/0.30</t>
+  </si>
+  <si>
+    <t>g0/0.35</t>
+  </si>
+  <si>
+    <t>g0/0.40</t>
+  </si>
+  <si>
+    <t>g0/0.95</t>
+  </si>
+  <si>
+    <t>130.45.128.1/26</t>
+  </si>
+  <si>
+    <t>130.45.128.65/26</t>
+  </si>
+  <si>
+    <t>130.45.128.129/26</t>
+  </si>
+  <si>
+    <t>130.45.128.193/26</t>
   </si>
 </sst>
 </file>
@@ -470,22 +494,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -805,7 +829,7 @@
   <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +932,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27.75" x14ac:dyDescent="0.4"/>
@@ -917,22 +941,22 @@
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="32"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="19" t="s">
@@ -1045,7 +1069,7 @@
     </row>
     <row r="8" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="9" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="31" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1059,6 +1083,15 @@
       <c r="C10" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="D10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="13">
@@ -1070,6 +1103,15 @@
       <c r="C11" s="15">
         <v>6</v>
       </c>
+      <c r="D11" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="22" t="s">
         <v>5</v>
       </c>
@@ -1084,6 +1126,15 @@
       <c r="C12" s="15">
         <v>12</v>
       </c>
+      <c r="D12" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="13">
@@ -1095,6 +1146,15 @@
       <c r="C13" s="15">
         <v>18</v>
       </c>
+      <c r="D13" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="16">
@@ -1105,6 +1165,15 @@
       </c>
       <c r="C14" s="18">
         <v>24</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>32</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>4</v>

</xml_diff>